<commit_message>
Issues #27 and #28
</commit_message>
<xml_diff>
--- a/inst/extdata/2.0.0/metadata/demo/ADAM_METADATA.xlsx
+++ b/inst/extdata/2.0.0/metadata/demo/ADAM_METADATA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\packages\defineR\inst\extdata\2.0.0\metadata\demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D67CDF14-037D-44F6-91DD-58B287466E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7D40500-5FB7-43C9-BAB9-035A07C8A85A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5130" windowWidth="29040" windowHeight="15840" tabRatio="900" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="38280" yWindow="5130" windowWidth="29040" windowHeight="15840" tabRatio="900"/>
   </bookViews>
   <sheets>
     <sheet name="DEFINE_HEADER_METADATA" sheetId="4" r:id="rId1"/>
@@ -2348,8 +2348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView zoomScale="106" zoomScaleNormal="106" zoomScalePageLayoutView="106" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" zoomScalePageLayoutView="106" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2433,7 +2433,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H65536"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2643,8 +2643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9888,7 +9888,7 @@
   <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>